<commit_message>
adding chart, tp growth signals
</commit_message>
<xml_diff>
--- a/Caxton/library/Good economists.xlsx
+++ b/Caxton/library/Good economists.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="23715" windowHeight="9630"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="23715" windowHeight="9630" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="good research and economist" sheetId="1" r:id="rId1"/>
+    <sheet name="brazil knowledge" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Good economist</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -87,6 +87,114 @@
   </si>
   <si>
     <t>Source</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>US Fixed Income Weekly</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB research</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sizing up the next phase of the Fed’s Treasury purchases</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BCB knowledge</t>
+  </si>
+  <si>
+    <t>selic: the average interest rates on interbank loans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPCA (Extended national cpi). </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>copom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Price index:</t>
+  </si>
+  <si>
+    <t>IPCA: reference for inflation targeting system.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INPC: 1-5 minimum wages bracket. </t>
+  </si>
+  <si>
+    <t>IPC: Fipe: income bracket 1 to 20.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPA:PPI (intercompany transactinos). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IGP-DI: industrial price?. IGP-M: released every 10 days. INCC: national index of construction cost. </t>
+  </si>
+  <si>
+    <t>IGP: price used for electricity.</t>
+  </si>
+  <si>
+    <t>subject</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>link</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BCB Monetary policy committee(copom)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>IPC-FIPE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Candara"/>
+        <family val="2"/>
+      </rPr>
+      <t>: calculated according to 30 day period ended every week.</t>
+    </r>
+  </si>
+  <si>
+    <t>inflation targeting system</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>primary instrument of monetary policy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brazilian FX swap</t>
+  </si>
+  <si>
+    <t>https://www.bcb.gov.br/en/financialstability/fxswap</t>
+  </si>
+  <si>
+    <t>https://www.elibrary.imf.org/view/IMF071/25455-9781484375686/25455-9781484375686/ch07.xml?language=en&amp;redirect=true</t>
+  </si>
+  <si>
+    <t>'Traditional' FX swaps </t>
+  </si>
+  <si>
+    <t>sale of U.S. dollars in the futures market. The other side will profit on BRL/USD higher</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>‘Reverse’ FX swaps</t>
+  </si>
+  <si>
+    <t>In case BRL under appreciation pressure</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -94,7 +202,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -155,6 +263,33 @@
       <name val="FrankRuehl"/>
       <family val="2"/>
       <charset val="177"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Candara"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Candara"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="8"/>
+      <color theme="10"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -183,7 +318,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -207,6 +342,27 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -216,6 +372,51 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3925259</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>257175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1026" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8573459" y="2543175"/>
+          <a:ext cx="1761166" cy="1085850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -505,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -541,7 +742,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="120">
+    <row r="3" spans="1:7" ht="60">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -558,7 +759,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="120">
+    <row r="4" spans="1:7" ht="48">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -573,7 +774,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="31.5">
+    <row r="5" spans="1:7" ht="21">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -612,7 +813,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="36">
+    <row r="8" spans="1:7" ht="24">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -627,10 +828,16 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+    <row r="9" spans="1:7" ht="24">
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="D9" s="2"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -654,14 +861,183 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.375" customWidth="1"/>
+    <col min="2" max="2" width="37.625" customWidth="1"/>
+    <col min="3" max="3" width="55.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="10"/>
+      <c r="B1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="10"/>
+    </row>
+    <row r="4" spans="1:3" ht="24">
+      <c r="A4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="10"/>
+    </row>
+    <row r="5" spans="1:3" ht="24">
+      <c r="A5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="10"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="10"/>
+    </row>
+    <row r="10" spans="1:3" ht="24">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="10"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="10"/>
+    </row>
+    <row r="12" spans="1:3" ht="24">
+      <c r="A12" s="10"/>
+      <c r="B12" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="10"/>
+    </row>
+    <row r="13" spans="1:3" ht="31.5" customHeight="1">
+      <c r="A13" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="33.75" customHeight="1">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+    </row>
+    <row r="16" spans="1:3" ht="28.5">
+      <c r="A16" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="10"/>
+    </row>
+    <row r="17" spans="1:3" ht="14.25">
+      <c r="A17" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="10"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C13" r:id="rId1"/>
+    <hyperlink ref="C14" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fed balance sheet insights
fed balance sheet insights
</commit_message>
<xml_diff>
--- a/Caxton/library/Good economists.xlsx
+++ b/Caxton/library/Good economists.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\yang\Third_yr_grad_English\relevant_file\workspace_zy\JY_completed\Caxton\library\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E9BBCD-1212-4356-ADEC-267158B6C25A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="23715" windowHeight="9630" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="good research and economist" sheetId="1" r:id="rId1"/>
@@ -201,19 +207,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -366,11 +372,19 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -391,7 +405,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1026" name="Picture 2"/>
+        <xdr:cNvPr id="1026" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -420,7 +440,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -462,7 +482,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -494,9 +514,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -528,6 +566,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -703,19 +759,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="21.125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="16.25" style="4" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="21.109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -742,7 +798,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="60">
+    <row r="3" spans="1:7" ht="68.400000000000006">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -759,7 +815,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="48">
+    <row r="4" spans="1:7" ht="57">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -774,7 +830,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="21">
+    <row r="5" spans="1:7" ht="19.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -787,7 +843,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="24">
+    <row r="6" spans="1:7" ht="22.8">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -800,7 +856,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" ht="31.5">
+    <row r="7" spans="1:7" ht="28.8">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -813,7 +869,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="24">
+    <row r="8" spans="1:7" ht="22.8">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -828,7 +884,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" ht="24">
+    <row r="9" spans="1:7" ht="34.200000000000003">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
@@ -846,13 +902,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="D3" r:id="rId3"/>
-    <hyperlink ref="C4" r:id="rId4"/>
-    <hyperlink ref="B5" r:id="rId5"/>
-    <hyperlink ref="B6" r:id="rId6"/>
-    <hyperlink ref="B7" r:id="rId7"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B6" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
@@ -860,18 +916,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.375" customWidth="1"/>
-    <col min="2" max="2" width="37.625" customWidth="1"/>
-    <col min="3" max="3" width="55.75" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
+    <col min="3" max="3" width="55.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -991,7 +1047,7 @@
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
     </row>
-    <row r="16" spans="1:3" ht="28.5">
+    <row r="16" spans="1:3" ht="28.8">
       <c r="A16" s="8" t="s">
         <v>44</v>
       </c>
@@ -1000,7 +1056,7 @@
       </c>
       <c r="C16" s="10"/>
     </row>
-    <row r="17" spans="1:3" ht="14.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="8" t="s">
         <v>46</v>
       </c>
@@ -1032,8 +1088,8 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C13" r:id="rId1"/>
-    <hyperlink ref="C14" r:id="rId2"/>
+    <hyperlink ref="C13" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C14" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -1042,12 +1098,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>